<commit_message>
changing AdvancedNuclear back to ConventionalNuclear
</commit_message>
<xml_diff>
--- a/inputs/ALEAF_inputs/ALEAF_IL_C2N.xlsx
+++ b/inputs/ALEAF_inputs/ALEAF_IL_C2N.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\biegelk\kb_aleaf\data\LC_GEP\IL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\biegelk\abce\inputs\ALEAF_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4068B88E-2AF5-443F-8ECE-E69E412F8727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666BE3B3-03F1-454C-B0C9-EF77167ECA43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="851" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -289,9 +289,6 @@
     <t>Nuclear</t>
   </si>
   <si>
-    <t>AdvancedNuclear</t>
-  </si>
-  <si>
     <t>bus_name</t>
   </si>
   <si>
@@ -494,6 +491,9 @@
   </si>
   <si>
     <t>Nuclear7</t>
+  </si>
+  <si>
+    <t>ConventionalNuclear</t>
   </si>
 </sst>
 </file>
@@ -1102,7 +1102,7 @@
   <dimension ref="A1:BD13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:F13"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1452,34 +1452,34 @@
     </row>
     <row r="4" spans="1:56">
       <c r="A4" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="B4" s="6">
-        <v>1</v>
-      </c>
-      <c r="C4" s="9" t="s">
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="D4" s="6">
-        <v>1</v>
-      </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>123</v>
-      </c>
       <c r="G4" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I4">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="J4" s="9">
-        <v>500</v>
+        <v>632</v>
       </c>
       <c r="K4" s="12">
         <v>0</v>
@@ -1713,13 +1713,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>83</v>
+        <v>151</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>82</v>
@@ -1742,25 +1742,25 @@
     </row>
     <row r="8" spans="1:56">
       <c r="A8" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="B8" s="6">
-        <v>1</v>
-      </c>
-      <c r="C8" s="9" t="s">
+      <c r="D8" s="6">
+        <v>1</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>128</v>
-      </c>
-      <c r="D8" s="6">
-        <v>1</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>129</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>82</v>
@@ -1783,25 +1783,25 @@
     </row>
     <row r="9" spans="1:56">
       <c r="A9" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="G9" s="9" t="s">
         <v>130</v>
-      </c>
-      <c r="B9" s="6">
-        <v>1</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="D9" s="6">
-        <v>1</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>131</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>82</v>
@@ -1824,25 +1824,25 @@
     </row>
     <row r="10" spans="1:56">
       <c r="A10" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B10" s="6">
         <v>1</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D10" s="6">
         <v>1</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>82</v>
@@ -1865,25 +1865,25 @@
     </row>
     <row r="11" spans="1:56">
       <c r="A11" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B11" s="6">
         <v>1</v>
       </c>
       <c r="C11" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>139</v>
-      </c>
-      <c r="D11" s="6">
-        <v>1</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>140</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>82</v>
@@ -1906,25 +1906,25 @@
     </row>
     <row r="12" spans="1:56">
       <c r="A12" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B12" s="6">
         <v>1</v>
       </c>
       <c r="C12" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>141</v>
-      </c>
-      <c r="D12" s="6">
-        <v>1</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>142</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>82</v>
@@ -1947,25 +1947,25 @@
     </row>
     <row r="13" spans="1:56">
       <c r="A13" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B13" s="6">
         <v>1</v>
       </c>
       <c r="C13" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D13" s="6">
+        <v>1</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G13" s="9" t="s">
         <v>143</v>
-      </c>
-      <c r="D13" s="6">
-        <v>1</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>144</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>82</v>
@@ -2012,37 +2012,37 @@
         <v>7</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -2050,13 +2050,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C2" s="6">
         <v>345</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E2" s="6">
         <v>89177</v>
@@ -2133,54 +2133,54 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" customHeight="1" thickBot="1">
       <c r="A1" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>110</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="6">
         <v>1</v>
@@ -2280,28 +2280,28 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
       <c r="A1" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>86</v>
-      </c>
       <c r="E1" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>91</v>
-      </c>
       <c r="H1" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2309,13 +2309,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C2" s="6">
         <v>345</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E2" s="6">
         <v>1</v>
@@ -2363,7 +2363,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2567,28 +2567,28 @@
     </row>
     <row r="2" spans="1:56">
       <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>115</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>116</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>117</v>
       </c>
-      <c r="F2" t="s">
-        <v>118</v>
-      </c>
       <c r="G2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2696,7 +2696,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -2731,28 +2731,28 @@
     </row>
     <row r="6" spans="1:56">
       <c r="A6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
         <v>120</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
         <v>121</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>122</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>123</v>
       </c>
-      <c r="G6" t="s">
-        <v>124</v>
-      </c>
       <c r="H6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I6">
         <v>29</v>
@@ -2790,7 +2790,7 @@
         <v>74</v>
       </c>
       <c r="G7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H7" t="s">
         <v>75</v>
@@ -2831,7 +2831,7 @@
         <v>79</v>
       </c>
       <c r="G8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H8" t="s">
         <v>75</v>
@@ -2872,7 +2872,7 @@
         <v>74</v>
       </c>
       <c r="G9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H9" t="s">
         <v>75</v>
@@ -2913,7 +2913,7 @@
         <v>79</v>
       </c>
       <c r="G10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H10" t="s">
         <v>75</v>
@@ -2954,7 +2954,7 @@
         <v>74</v>
       </c>
       <c r="G11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H11" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
adding 2 AdvancedNuclear units to the IL portfolio (agent 201)
</commit_message>
<xml_diff>
--- a/inputs/ALEAF_inputs/ALEAF_IL_C2N.xlsx
+++ b/inputs/ALEAF_inputs/ALEAF_IL_C2N.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\biegelk\abce\inputs\ALEAF_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666BE3B3-03F1-454C-B0C9-EF77167ECA43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5036DC-4833-4F89-AA06-CBA31DD02D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="851" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="156">
   <si>
     <t>Setting</t>
   </si>
@@ -494,6 +494,18 @@
   </si>
   <si>
     <t>ConventionalNuclear</t>
+  </si>
+  <si>
+    <t>1_nuclear_8</t>
+  </si>
+  <si>
+    <t>Tech17</t>
+  </si>
+  <si>
+    <t>Nuclear8</t>
+  </si>
+  <si>
+    <t>AdvancedNuclear</t>
   </si>
 </sst>
 </file>
@@ -1099,10 +1111,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:BD13"/>
+  <dimension ref="A1:BD14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1725,7 +1737,7 @@
         <v>82</v>
       </c>
       <c r="I7">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J7" s="9">
         <v>300</v>
@@ -1983,6 +1995,47 @@
         <v>0</v>
       </c>
       <c r="M13" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:56">
+      <c r="A14" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B14" s="6">
+        <v>1</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="J14" s="9">
+        <v>300</v>
+      </c>
+      <c r="K14" s="12">
+        <v>0</v>
+      </c>
+      <c r="L14" s="12">
+        <v>0</v>
+      </c>
+      <c r="M14" s="12">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
removing 5 extraneous NGCC from the system
</commit_message>
<xml_diff>
--- a/inputs/ALEAF_inputs/ALEAF_IL_C2N.xlsx
+++ b/inputs/ALEAF_inputs/ALEAF_IL_C2N.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\biegelk\abce\inputs\ALEAF_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5036DC-4833-4F89-AA06-CBA31DD02D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966915E3-6193-4B3C-A5AF-E5CCA3ACEC4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="851" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1114,7 +1114,7 @@
   <dimension ref="A1:BD14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1571,7 +1571,7 @@
         <v>75</v>
       </c>
       <c r="I5">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="J5" s="9">
         <v>200</v>

</xml_diff>